<commit_message>
test to update ghost line
</commit_message>
<xml_diff>
--- a/marelli_data_complete.xlsx
+++ b/marelli_data_complete.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA16"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -699,13 +699,41 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FIASA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>800000055</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MARELLI SISTEMAS</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Robson Cassemiro</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Isabela Santos</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>250325</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Limited capacity at Marelli supplier in order attend 770 JPD of Stellantis. Duplicate the Final Assembly line.</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>2</t>
@@ -774,393 +802,153 @@
         </is>
       </c>
       <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Maria Eduarda</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>André Albuquerque</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Ivan Anjos</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Victor Gonçaves Souza</t>
+        </is>
+      </c>
       <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FIASA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>800000055</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MARELLI SISTEMAS</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Robson Cassemiro</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Isabela Santos</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>250325</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Limited capacity at Marelli supplier in order attend 770 JPD of Stellantis. Duplicate the Final Assembly line.</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>​</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>5,4</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>620</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>3452</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>5,4</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>4368</t>
+        </is>
+      </c>
       <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Maria Eduarda</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>André Albuquerque</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Ivan Anjos</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Victor Gonçaves Souza</t>
+        </is>
+      </c>
       <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>​</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>